<commit_message>
Added field for Prefault time
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/SmokeTestData.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/SmokeTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C0D80A-0FF2-4085-B465-9883F932BC35}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248D2D07-E630-4C32-9AA8-59D260089C6F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>DeviceName</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t>409026540</t>
+  </si>
+  <si>
+    <t>PrefaultTime</t>
+  </si>
+  <si>
+    <t>2569</t>
   </si>
 </sst>
 </file>
@@ -371,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -387,7 +393,7 @@
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -406,8 +412,11 @@
       <c r="F1" t="s">
         <v>8</v>
       </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -425,6 +434,9 @@
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the Dataset file to use device 53 instead of 51
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/SmokeTestData.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/SmokeTestData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248D2D07-E630-4C32-9AA8-59D260089C6F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EDDB6F-4011-4638-B044-2F98BCF9A851}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,15 +28,9 @@
     <t>DeviceType</t>
   </si>
   <si>
-    <t>IND_DAU_51</t>
-  </si>
-  <si>
     <t>IDM+18</t>
   </si>
   <si>
-    <t>10.75.58.51</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
@@ -52,13 +46,19 @@
     <t>DeviceIPAdd</t>
   </si>
   <si>
-    <t>409026540</t>
-  </si>
-  <si>
     <t>PrefaultTime</t>
   </si>
   <si>
     <t>2569</t>
+  </si>
+  <si>
+    <t>10.75.58.53</t>
+  </si>
+  <si>
+    <t>IND_DAU_53</t>
+  </si>
+  <si>
+    <t>390553122</t>
   </si>
 </sst>
 </file>
@@ -380,7 +380,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,10 +395,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -407,36 +407,36 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated excel file for device 51
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/SmokeTestData.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/SmokeTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EDDB6F-4011-4638-B044-2F98BCF9A851}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DBE7AE08-7213-44B8-A36A-124F2B7B8C08}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>DeviceName</t>
   </si>
@@ -52,13 +52,10 @@
     <t>2569</t>
   </si>
   <si>
-    <t>10.75.58.53</t>
-  </si>
-  <si>
-    <t>IND_DAU_53</t>
-  </si>
-  <si>
-    <t>390553122</t>
+    <t>IND_DAU_51</t>
+  </si>
+  <si>
+    <t>10.75.58.51</t>
   </si>
 </sst>
 </file>
@@ -380,20 +377,20 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -416,7 +413,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -424,16 +421,16 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="F2" s="1">
+        <v>409026540</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>9</v>
@@ -441,5 +438,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AIP-68-AIP-272 Added one more column of Post fault time
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/SmokeTestData.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/SmokeTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DBE7AE08-7213-44B8-A36A-124F2B7B8C08}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B0FDE7-6079-443C-8C68-A2C9A071567B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>DeviceName</t>
   </si>
@@ -56,6 +56,12 @@
   </si>
   <si>
     <t>10.75.58.51</t>
+  </si>
+  <si>
+    <t>PostFaultTime</t>
+  </si>
+  <si>
+    <t>530</t>
   </si>
 </sst>
 </file>
@@ -374,23 +380,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -412,8 +419,11 @@
       <c r="G1" t="s">
         <v>8</v>
       </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -434,6 +444,9 @@
       </c>
       <c r="G2" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AIP-68 AIP-273 Updated Test Data Added Fields for Voltage and current injection
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/SmokeTestData.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/SmokeTestData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B0FDE7-6079-443C-8C68-A2C9A071567B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3D2CDA-FD9A-4F01-89D6-41EF9F6F6C6E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>DeviceName</t>
   </si>
@@ -62,6 +62,18 @@
   </si>
   <si>
     <t>530</t>
+  </si>
+  <si>
+    <t>RMSInjectedVoltage</t>
+  </si>
+  <si>
+    <t>RMSInjectedCurrent</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -380,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,9 +407,12 @@
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -422,8 +437,14 @@
       <c r="H1" t="s">
         <v>12</v>
       </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -447,6 +468,12 @@
       </c>
       <c r="H2" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AIP-68 AIP-365 TestData For Manual DFR
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/SmokeTestData.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/SmokeTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3D2CDA-FD9A-4F01-89D6-41EF9F6F6C6E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D467F923-B1CE-4A40-9067-C173C5870B77}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>DeviceName</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>OmicronFile</t>
+  </si>
+  <si>
+    <t>ManualDFRInjection.qcm</t>
   </si>
 </sst>
 </file>
@@ -392,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,7 +418,7 @@
     <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -443,8 +449,11 @@
       <c r="J1" t="s">
         <v>15</v>
       </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -474,6 +483,9 @@
       </c>
       <c r="J2" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AIP-306 AIP-353 Added Set Max DFR for existing script
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/SmokeTestData.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/SmokeTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D467F923-B1CE-4A40-9067-C173C5870B77}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D127B2FF-7C9F-4535-AB1B-3F3F51F238C4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>DeviceName</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>ManualDFRInjection.qcm</t>
+  </si>
+  <si>
+    <t>MaxDFR</t>
+  </si>
+  <si>
+    <t>5000</t>
   </si>
 </sst>
 </file>
@@ -398,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,9 +422,10 @@
     <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -452,8 +459,11 @@
       <c r="K1" t="s">
         <v>18</v>
       </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -486,6 +496,9 @@
       </c>
       <c r="K2" t="s">
         <v>19</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>